<commit_message>
added public form logic
</commit_message>
<xml_diff>
--- a/assets/projects-invoice-cess-template/projects-invoices-cess-template.xlsx
+++ b/assets/projects-invoice-cess-template/projects-invoices-cess-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\CORE-MBOCW-CESS\assets\projects-invoice-cess-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFD12B9-F852-4A8A-8B2F-A92A55372D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51027291-5B8D-4F29-A75A-4A7B97B75B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{67C406E2-A0AD-4F41-8350-A439232F5AFF}"/>
   </bookViews>
@@ -126,9 +126,6 @@
     <t xml:space="preserve">Slum Rehabilitation  </t>
   </si>
   <si>
-    <t>Gov. Org</t>
-  </si>
-  <si>
     <t>Employer Name 2</t>
   </si>
   <si>
@@ -346,6 +343,9 @@
   </si>
   <si>
     <t>employer10@gmail.com</t>
+  </si>
+  <si>
+    <t>Government Organization</t>
   </si>
 </sst>
 </file>
@@ -353,7 +353,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -890,7 +890,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -920,8 +920,7 @@
     <xf numFmtId="0" fontId="16" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1280,9 +1279,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
+      <selection pane="bottomLeft" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1310,7 +1309,7 @@
     <col min="48" max="48" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="55.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1391,7 +1390,7 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
         <v>23</v>
@@ -1434,7 +1433,7 @@
         <v>5073.75</v>
       </c>
       <c r="Q2" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="R2" t="s">
         <v>25</v>
@@ -1449,7 +1448,7 @@
         <v>123456789</v>
       </c>
       <c r="AV2" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AX2" s="8" t="s">
         <v>27</v>
@@ -1461,7 +1460,7 @@
         <v>13</v>
       </c>
       <c r="BD2" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.3">
@@ -1472,13 +1471,13 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3">
         <v>500000</v>
@@ -1521,10 +1520,10 @@
         <v>24</v>
       </c>
       <c r="R3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" t="s">
         <v>32</v>
-      </c>
-      <c r="S3" t="s">
-        <v>33</v>
       </c>
       <c r="T3">
         <v>1234568970</v>
@@ -1533,19 +1532,19 @@
         <v>555656565</v>
       </c>
       <c r="AV3" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AX3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ3" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AZ3" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="BB3" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="BD3" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.3">
@@ -1553,16 +1552,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4">
         <v>4500000</v>
@@ -1605,10 +1604,10 @@
         <v>24</v>
       </c>
       <c r="R4" t="s">
+        <v>38</v>
+      </c>
+      <c r="S4" t="s">
         <v>39</v>
-      </c>
-      <c r="S4" t="s">
-        <v>40</v>
       </c>
       <c r="T4">
         <v>8523697410</v>
@@ -1617,19 +1616,19 @@
         <v>562315478</v>
       </c>
       <c r="AV4" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AX4" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AZ4" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BB4" s="9" t="s">
         <v>24</v>
       </c>
       <c r="BD4" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.3">
@@ -1637,16 +1636,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5">
         <v>900000</v>
@@ -1689,10 +1688,10 @@
         <v>24</v>
       </c>
       <c r="R5" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" t="s">
         <v>43</v>
-      </c>
-      <c r="S5" t="s">
-        <v>44</v>
       </c>
       <c r="T5">
         <v>2310564798</v>
@@ -1704,16 +1703,16 @@
         <v>29</v>
       </c>
       <c r="AX5" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AZ5" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="BB5" s="9" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="BD5" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.3">
@@ -1721,16 +1720,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6">
         <v>1700000</v>
@@ -1773,10 +1772,10 @@
         <v>24</v>
       </c>
       <c r="R6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" t="s">
         <v>47</v>
-      </c>
-      <c r="S6" t="s">
-        <v>48</v>
       </c>
       <c r="T6">
         <v>6932051847</v>
@@ -1785,13 +1784,13 @@
         <v>562315478</v>
       </c>
       <c r="AV6" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AX6" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AZ6" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.3">
@@ -1799,16 +1798,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F7">
         <v>4500000</v>
@@ -1851,10 +1850,10 @@
         <v>24</v>
       </c>
       <c r="R7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S7" t="s">
         <v>52</v>
-      </c>
-      <c r="S7" t="s">
-        <v>53</v>
       </c>
       <c r="T7">
         <v>4895126370</v>
@@ -1863,13 +1862,13 @@
         <v>562315478</v>
       </c>
       <c r="AV7" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AX7" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AZ7" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.3">
@@ -1877,16 +1876,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F8">
         <v>600000</v>
@@ -1929,10 +1928,10 @@
         <v>24</v>
       </c>
       <c r="R8" t="s">
+        <v>55</v>
+      </c>
+      <c r="S8" t="s">
         <v>56</v>
-      </c>
-      <c r="S8" t="s">
-        <v>57</v>
       </c>
       <c r="T8">
         <v>7534210869</v>
@@ -1941,10 +1940,10 @@
         <v>562315478</v>
       </c>
       <c r="AX8" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AZ8" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.3">
@@ -1952,16 +1951,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" t="s">
         <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F9">
         <v>550000</v>
@@ -2004,10 +2003,10 @@
         <v>24</v>
       </c>
       <c r="R9" t="s">
+        <v>59</v>
+      </c>
+      <c r="S9" t="s">
         <v>60</v>
-      </c>
-      <c r="S9" t="s">
-        <v>61</v>
       </c>
       <c r="T9">
         <v>8695742310</v>
@@ -2016,10 +2015,10 @@
         <v>562315478</v>
       </c>
       <c r="AX9" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AZ9" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.3">
@@ -2027,16 +2026,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F10">
         <v>600000</v>
@@ -2079,10 +2078,10 @@
         <v>24</v>
       </c>
       <c r="R10" t="s">
+        <v>64</v>
+      </c>
+      <c r="S10" t="s">
         <v>65</v>
-      </c>
-      <c r="S10" t="s">
-        <v>66</v>
       </c>
       <c r="T10">
         <v>2630154897</v>
@@ -2091,10 +2090,10 @@
         <v>562315478</v>
       </c>
       <c r="AX10" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AZ10" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.3">
@@ -2102,16 +2101,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
         <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F11">
         <v>4500000</v>
@@ -2151,13 +2150,13 @@
         <v>8118</v>
       </c>
       <c r="Q11" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="R11" t="s">
+        <v>102</v>
+      </c>
+      <c r="S11" t="s">
         <v>103</v>
-      </c>
-      <c r="S11" s="14" t="s">
-        <v>104</v>
       </c>
       <c r="T11">
         <v>5689457826</v>
@@ -2166,50 +2165,50 @@
         <v>895647125</v>
       </c>
       <c r="AX11" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AZ11" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.3">
       <c r="AX12" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AZ12" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:56" x14ac:dyDescent="0.3">
       <c r="AX13" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AZ13" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.3">
       <c r="AX14" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AZ14" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.3">
       <c r="AX15" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AZ15" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.3">
       <c r="AX16" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AZ16" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="50:52" x14ac:dyDescent="0.3">
@@ -2217,15 +2216,15 @@
         <v>30</v>
       </c>
       <c r="AZ17" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="50:52" x14ac:dyDescent="0.3">
       <c r="AX18" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AZ18" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="50:52" x14ac:dyDescent="0.3">
@@ -2233,37 +2232,37 @@
         <v>22</v>
       </c>
       <c r="AZ19" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="50:52" x14ac:dyDescent="0.3">
       <c r="AZ20" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="50:52" x14ac:dyDescent="0.3">
       <c r="AZ21" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="50:52" x14ac:dyDescent="0.3">
       <c r="AZ22" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="50:52" x14ac:dyDescent="0.3">
       <c r="AZ23" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="50:52" x14ac:dyDescent="0.3">
       <c r="AZ24" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="50:52" x14ac:dyDescent="0.3">
       <c r="AZ25" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>